<commit_message>
Flashcards aus DB anzeigen
</commit_message>
<xml_diff>
--- a/Sprint.xlsx
+++ b/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FlashLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C617153-1745-4BF9-A909-CAB7437E1EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED3B811-83E6-4B08-9AAE-293EEBF30ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="9825" yWindow="3300" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Fehlerbehebung</t>
+  </si>
+  <si>
+    <t>Flashcards aus DB anzeigen lassen</t>
   </si>
 </sst>
 </file>
@@ -508,6 +511,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,12 +551,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -545,27 +569,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -982,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -999,28 +1002,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1034,133 +1037,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1356,6 +1359,442 @@
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
         <v>0.79999999999999982</v>
+      </c>
+      <c r="F26" s="6">
+        <f>COUNT(F16:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <f>COUNT(G16:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H16" r:id="rId1" xr:uid="{FEA80941-257C-4BA0-B607-B95F875549EB}"/>
+    <hyperlink ref="H17" r:id="rId2" xr:uid="{B7E10C11-7F0F-4CB1-8924-2DB26C84E386}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75D9A9F-E52D-4D98-8268-AFECBCBC2104}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
+        <v>2</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
+        <v>11</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <f>D16-C16</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>5</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17-C17</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>7</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2">
+        <f>D22-C22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2">
+        <f>D23-C23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2">
+        <f>D24-C24</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2">
+        <f>D25-C25</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f>SUM(E16:E25)</f>
+        <v>4</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -1400,442 +1839,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="H16" r:id="rId1" xr:uid="{FEA80941-257C-4BA0-B607-B95F875549EB}"/>
-    <hyperlink ref="H17" r:id="rId2" xr:uid="{B7E10C11-7F0F-4CB1-8924-2DB26C84E386}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75D9A9F-E52D-4D98-8268-AFECBCBC2104}">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="2"/>
-    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
-        <v>2</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>4</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="7">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7">
-        <v>3</v>
-      </c>
-      <c r="E16" s="2">
-        <f>D16-C16</f>
-        <v>1</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>5</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="7">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2">
-        <f>D17-C17</f>
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>6</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="7">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7">
-        <v>2.5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="2">
-        <v>3</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2">
-        <f>D22-C22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
-        <f>D23-C23</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2">
-        <f>D24-C24</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2">
-        <f>D25-C25</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <f>SUM(E16:E25)</f>
-        <v>4</v>
-      </c>
-      <c r="F26" s="6">
-        <f>COUNT(F16:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f>COUNT(G16:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1863,28 +1866,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1898,133 +1901,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>3</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2258,6 +2261,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -2273,11 +2281,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2288,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8D5CB8-688E-4936-A911-D91BEAE18A84}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2305,28 +2308,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2340,133 +2343,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2688,6 +2691,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:G10"/>
@@ -2695,19 +2711,6 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2735,28 +2738,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2770,133 +2773,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>5</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3136,6 +3139,447 @@
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
         <v>8</v>
+      </c>
+      <c r="F26" s="6">
+        <f>COUNT(F16:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <f>COUNT(G16:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
+        <v>6</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
+        <v>11</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2">
+        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
+        <v>-3</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>21</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="7">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2">
+        <f>D21-C21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2">
+        <f>D22-C22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f>SUM(E16:E25)</f>
+        <v>-8</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -3183,436 +3627,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="2"/>
-    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
-        <v>6</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2">
-        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
-        <v>-3</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="7">
-        <v>5</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>21</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="7">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>22</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="2">
-        <f>D21-C21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2">
-        <f>D22-C22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <f>SUM(E16:E25)</f>
-        <v>-11</v>
-      </c>
-      <c r="F26" s="6">
-        <f>COUNT(F16:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f>COUNT(G16:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Flashcard in DB speichern
</commit_message>
<xml_diff>
--- a/Sprint.xlsx
+++ b/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FlashLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2C56F2-1B76-41DC-AE56-BEB80E3563D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2E039-2943-4DE0-8D1A-535B33F962E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9825" yWindow="3300" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="5535" yWindow="2295" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="71">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Flashcards aus DB anzeigen lassen</t>
+  </si>
+  <si>
+    <t>Add Flashcard in DB speichern</t>
   </si>
 </sst>
 </file>
@@ -511,6 +514,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,12 +554,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -548,27 +572,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1002,28 +1005,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1037,133 +1040,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1383,12 +1386,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1403,6 +1400,12 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H16" r:id="rId1" xr:uid="{FEA80941-257C-4BA0-B607-B95F875549EB}"/>
@@ -1434,28 +1437,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1469,133 +1472,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>2</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1819,6 +1822,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1833,12 +1842,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1866,28 +1869,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1901,133 +1904,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>3</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2261,6 +2264,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -2276,11 +2284,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2308,28 +2311,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2343,133 +2346,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2691,6 +2694,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:G10"/>
@@ -2698,19 +2714,6 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2738,28 +2741,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2773,133 +2776,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>5</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3139,6 +3142,455 @@
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
         <v>8</v>
+      </c>
+      <c r="F26" s="6">
+        <f>COUNT(F16:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <f>COUNT(G16:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
+        <v>6</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
+        <v>11</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2">
+        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
+        <v>-3</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>21</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="7">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <f>D21-C21</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2">
+        <f>D22-C22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f>SUM(E16:E25)</f>
+        <v>-6</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -3186,446 +3638,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="2"/>
-    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
-        <v>6</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2">
-        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
-        <v>-3</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="7">
-        <v>5</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>21</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="7">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>22</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>23</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="7">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="2">
-        <f>D21-C21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2">
-        <f>D22-C22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <f>SUM(E16:E25)</f>
-        <v>-8</v>
-      </c>
-      <c r="F26" s="6">
-        <f>COUNT(F16:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f>COUNT(G16:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit Flashcard in DB speichern
</commit_message>
<xml_diff>
--- a/Sprint.xlsx
+++ b/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FlashLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2E039-2943-4DE0-8D1A-535B33F962E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA67FB-3B4D-4883-AB3F-5A3729C1A45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="2295" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="7605" yWindow="4305" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="72">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Add Flashcard in DB speichern</t>
+  </si>
+  <si>
+    <t>Edit Flashcard in DB speichern</t>
   </si>
 </sst>
 </file>
@@ -514,33 +517,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,6 +530,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,6 +554,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1005,28 +1008,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1040,133 +1043,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17">
         <v>1</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="26">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
         <v>11</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1386,6 +1389,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1400,12 +1409,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H16" r:id="rId1" xr:uid="{FEA80941-257C-4BA0-B607-B95F875549EB}"/>
@@ -1437,28 +1440,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1472,133 +1475,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17">
         <v>2</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="26">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
         <v>11</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1822,12 +1825,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1842,6 +1839,12 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1869,28 +1872,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1904,133 +1907,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17">
         <v>3</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="26">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
         <v>11</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2264,11 +2267,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -2284,6 +2282,11 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2311,28 +2314,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2346,133 +2349,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17">
         <v>4</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="26">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
         <v>11</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2694,6 +2697,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="A1:I2"/>
@@ -2701,19 +2717,6 @@
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2741,28 +2744,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2776,133 +2779,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17">
         <v>5</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="26">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
         <v>11</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3142,6 +3145,463 @@
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
         <v>8</v>
+      </c>
+      <c r="F26" s="6">
+        <f>COUNT(F16:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <f>COUNT(G16:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="17">
+        <v>6</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2">
+        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
+        <v>-3</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>21</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="7">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <f>D21-C21</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>25</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="7">
+        <v>3</v>
+      </c>
+      <c r="D22" s="7">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <f>D22-C22</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f>SUM(E16:E25)</f>
+        <v>-4</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -3189,454 +3649,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="2"/>
-    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
-        <v>6</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="26">
-        <v>11</v>
-      </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2">
-        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
-        <v>-3</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="7">
-        <v>5</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>21</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="7">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>22</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>23</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="7">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>24</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="7">
-        <v>3</v>
-      </c>
-      <c r="D21" s="7">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <f>D21-C21</f>
-        <v>2</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2">
-        <f>D22-C22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <f>SUM(E16:E25)</f>
-        <v>-6</v>
-      </c>
-      <c r="F26" s="6">
-        <f>COUNT(F16:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f>COUNT(G16:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delete Flashcard in DB speichern
</commit_message>
<xml_diff>
--- a/Sprint.xlsx
+++ b/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FlashLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA67FB-3B4D-4883-AB3F-5A3729C1A45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C13A7BA-76B0-4C94-92AA-0610B39DA20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="4305" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="7230" yWindow="3690" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="73">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Edit Flashcard in DB speichern</t>
+  </si>
+  <si>
+    <t>Delete Flashcard in DB speichern</t>
   </si>
 </sst>
 </file>
@@ -517,6 +520,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -530,12 +560,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -554,27 +578,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1008,28 +1011,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1043,133 +1046,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1389,12 +1392,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1409,6 +1406,12 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H16" r:id="rId1" xr:uid="{FEA80941-257C-4BA0-B607-B95F875549EB}"/>
@@ -1440,28 +1443,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1475,133 +1478,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>2</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1825,6 +1828,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1839,12 +1848,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1872,28 +1875,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -1907,133 +1910,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>3</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2267,6 +2270,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -2282,11 +2290,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2314,28 +2317,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2349,133 +2352,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2697,6 +2700,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:G10"/>
@@ -2704,19 +2720,6 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2744,28 +2747,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -2779,133 +2782,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>5</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
         <v>11</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3145,6 +3148,471 @@
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
         <v>8</v>
+      </c>
+      <c r="F26" s="6">
+        <f>COUNT(F16:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <f>COUNT(G16:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
+        <v>6</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="26">
+        <v>11</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2">
+        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
+        <v>-3</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>21</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="7">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <f>D21-C21</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>25</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="7">
+        <v>3</v>
+      </c>
+      <c r="D22" s="7">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <f>D22-C22</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2</v>
+      </c>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <f>SUM(E16:E25)</f>
+        <v>-1</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -3192,462 +3660,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D6D64-D230-499F-9E8D-DCE0DA1676D8}">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="2"/>
-    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
-        <v>6</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2">
-        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
-        <v>-3</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="7">
-        <v>5</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>21</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="7">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>22</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>23</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="7">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>24</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="7">
-        <v>3</v>
-      </c>
-      <c r="D21" s="7">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <f>D21-C21</f>
-        <v>2</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>25</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="7">
-        <v>3</v>
-      </c>
-      <c r="D22" s="7">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <f>D22-C22</f>
-        <v>2</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <f>SUM(E16:E25)</f>
-        <v>-4</v>
-      </c>
-      <c r="F26" s="6">
-        <f>COUNT(F16:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <f>COUNT(G16:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
redundanten Code entfernt; Protokoll angepasst
</commit_message>
<xml_diff>
--- a/Sprint.xlsx
+++ b/Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FlashLearn\FlashLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96849B96-B8F4-4997-AAB1-3AA879513FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E862A4-5C49-4876-AA5C-9609413E7D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="119">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>Kategorieansicht</t>
+  </si>
+  <si>
+    <t>redundanten Code entfernt</t>
   </si>
 </sst>
 </file>
@@ -3829,7 +3832,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4793,15 +4796,25 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="8"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="A56" s="8">
+        <v>47</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E56" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G56" s="4"/>
       <c r="H56" s="7"/>
     </row>

</xml_diff>

<commit_message>
Creation of the logo image (without AI) and adding it to the header
</commit_message>
<xml_diff>
--- a/Sprint.xlsx
+++ b/Sprint.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninas\Documents\Uni\2. Semester (SS 2025)\IT Projekt\Artefacts\protocols\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natyd\Desktop\ITP_SS25\Flashlerarn\FlashLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A66E7F-AE60-4CDF-8B1D-75F4E21B145E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFF29DA-A9A0-4EDF-A448-CA07D7C7B022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_1" sheetId="1" r:id="rId1"/>
@@ -21,28 +21,17 @@
     <sheet name="Sprint_6" sheetId="14" r:id="rId6"/>
     <sheet name="Sprint_7" sheetId="15" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="123">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -402,6 +391,15 @@
   </si>
   <si>
     <t>29.06.2025</t>
+  </si>
+  <si>
+    <t>Ortiz Arias,Silvia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellung des Logobildes (ohne KI) </t>
+  </si>
+  <si>
+    <t>und Einfügen in den Header</t>
   </si>
 </sst>
 </file>
@@ -731,8 +729,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -845,9 +843,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -885,7 +883,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -991,7 +989,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1133,7 +1131,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1147,19 +1145,19 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="32.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1170,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1183,7 +1181,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1194,7 +1192,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -1207,7 +1205,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -1220,7 +1218,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -1233,7 +1231,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -1246,7 +1244,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1257,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1270,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -1285,7 +1283,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1296,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -1311,7 +1309,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1321,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1349,7 +1347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -1374,7 +1372,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>2</v>
       </c>
@@ -1399,7 +1397,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>3</v>
       </c>
@@ -1421,7 +1419,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1433,7 +1431,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1445,7 +1443,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1457,7 +1455,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1470,7 +1468,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1483,7 +1481,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1496,7 +1494,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1509,7 +1507,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1528,13 +1526,13 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -1579,19 +1577,19 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="32.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1602,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1615,7 +1613,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1626,7 +1624,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -1639,7 +1637,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -1652,7 +1650,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -1665,7 +1663,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -1678,7 +1676,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -1691,7 +1689,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -1704,7 +1702,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -1717,7 +1715,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -1730,7 +1728,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -1743,7 +1741,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -1755,7 +1753,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1781,7 +1779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>4</v>
       </c>
@@ -1804,7 +1802,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>5</v>
       </c>
@@ -1827,7 +1825,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>6</v>
       </c>
@@ -1849,7 +1847,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>7</v>
       </c>
@@ -1869,7 +1867,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1881,7 +1879,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1893,7 +1891,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1906,7 +1904,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1919,7 +1917,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1932,7 +1930,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1945,7 +1943,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1964,13 +1962,13 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -2011,19 +2009,19 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="32.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2036,7 +2034,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2047,7 +2045,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2058,7 +2056,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -2071,7 +2069,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -2084,7 +2082,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -2097,7 +2095,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -2110,7 +2108,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -2123,7 +2121,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2134,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -2149,7 +2147,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -2162,7 +2160,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -2175,7 +2173,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -2187,7 +2185,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2213,7 +2211,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>7</v>
       </c>
@@ -2236,7 +2234,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>8</v>
       </c>
@@ -2259,7 +2257,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>9</v>
       </c>
@@ -2282,7 +2280,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>10</v>
       </c>
@@ -2299,7 +2297,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>11</v>
       </c>
@@ -2322,7 +2320,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2335,7 +2333,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2348,7 +2346,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2361,7 +2359,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -2374,7 +2372,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -2387,7 +2385,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2406,13 +2404,13 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -2453,19 +2451,19 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="32.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2478,7 +2476,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2489,7 +2487,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2500,7 +2498,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -2513,7 +2511,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -2526,7 +2524,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -2539,7 +2537,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -2552,7 +2550,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -2565,7 +2563,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -2578,7 +2576,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -2591,7 +2589,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -2604,7 +2602,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -2617,7 +2615,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -2629,7 +2627,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>12</v>
       </c>
@@ -2678,7 +2676,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="7" t="s">
         <v>45</v>
@@ -2693,7 +2691,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>15</v>
       </c>
@@ -2716,7 +2714,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>10</v>
       </c>
@@ -2739,7 +2737,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2752,7 +2750,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2765,7 +2763,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2778,7 +2776,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2791,7 +2789,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -2804,7 +2802,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -2817,7 +2815,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -2836,13 +2834,13 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -2883,19 +2881,19 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="32.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2908,7 +2906,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2919,7 +2917,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2930,7 +2928,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -2943,7 +2941,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -2956,7 +2954,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -2969,7 +2967,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -2982,7 +2980,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -2995,7 +2993,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -3008,7 +3006,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -3021,7 +3019,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -3034,7 +3032,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -3047,7 +3045,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +3057,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -3085,7 +3083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>13</v>
       </c>
@@ -3110,7 +3108,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -3125,7 +3123,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3140,7 +3138,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -3163,7 +3161,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -3188,7 +3186,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -3213,7 +3211,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -3238,7 +3236,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -3263,7 +3261,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3276,7 +3274,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -3289,7 +3287,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -3308,13 +3306,13 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3356,19 +3354,19 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="33.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3379,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -3392,7 +3390,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3403,7 +3401,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -3416,7 +3414,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -3429,7 +3427,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -3442,7 +3440,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +3453,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -3468,7 +3466,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -3481,7 +3479,7 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -3494,7 +3492,7 @@
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -3507,7 +3505,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -3520,7 +3518,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -3532,7 +3530,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -3558,7 +3556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>19</v>
       </c>
@@ -3579,7 +3577,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>20</v>
       </c>
@@ -3600,7 +3598,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>21</v>
       </c>
@@ -3621,7 +3619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>22</v>
       </c>
@@ -3644,7 +3642,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>23</v>
       </c>
@@ -3667,7 +3665,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>24</v>
       </c>
@@ -3690,7 +3688,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>25</v>
       </c>
@@ -3713,7 +3711,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>26</v>
       </c>
@@ -3736,7 +3734,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>27</v>
       </c>
@@ -3759,7 +3757,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -3772,7 +3770,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -3791,13 +3789,13 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3834,23 +3832,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF89246-3E12-4BB9-8AB6-B155DC5DC5C8}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="119" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="36.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="2"/>
+    <col min="2" max="2" width="41.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="36.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3863,7 +3861,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -3874,7 +3872,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3885,7 +3883,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -3898,7 +3896,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -3911,7 +3909,7 @@
       <c r="F5" s="31"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -3924,7 +3922,7 @@
       <c r="F6" s="31"/>
       <c r="G6" s="32"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -3937,7 +3935,7 @@
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -3950,7 +3948,7 @@
       <c r="F8" s="25"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -3963,18 +3961,20 @@
       <c r="F9" s="25"/>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="18"/>
-      <c r="C10" s="25"/>
+      <c r="C10" s="25" t="s">
+        <v>120</v>
+      </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -3985,7 +3985,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -4010,7 +4010,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>28</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>29</v>
       </c>
@@ -4082,7 +4082,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="7" t="s">
         <v>76</v>
@@ -4097,7 +4097,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>30</v>
       </c>
@@ -4120,7 +4120,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>31</v>
       </c>
@@ -4143,7 +4143,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="7" t="s">
         <v>82</v>
@@ -4158,7 +4158,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>32</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="7" t="s">
         <v>82</v>
@@ -4196,7 +4196,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>33</v>
       </c>
@@ -4219,7 +4219,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="7" t="s">
         <v>79</v>
@@ -4234,7 +4234,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="7" t="s">
         <v>80</v>
@@ -4249,7 +4249,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>34</v>
       </c>
@@ -4270,7 +4270,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="7" t="s">
         <v>85</v>
@@ -4285,7 +4285,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>35</v>
       </c>
@@ -4306,7 +4306,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="7" t="s">
         <v>87</v>
@@ -4321,7 +4321,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>36</v>
       </c>
@@ -4342,7 +4342,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>37</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="7" t="s">
         <v>90</v>
@@ -4382,7 +4382,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="7" t="s">
         <v>91</v>
@@ -4397,7 +4397,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="7" t="s">
         <v>92</v>
@@ -4412,7 +4412,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>38</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -4452,7 +4452,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -4467,7 +4467,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -4482,7 +4482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>39</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -4522,7 +4522,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>40</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -4562,7 +4562,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>41</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" ref="E44:E58" si="3">D44-C44</f>
+        <f t="shared" ref="E44:E57" si="3">D44-C44</f>
         <v>0</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -4587,7 +4587,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -4602,7 +4602,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -4617,7 +4617,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>42</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -4657,7 +4657,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -4672,7 +4672,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>43</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>44</v>
       </c>
@@ -4718,7 +4718,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>45</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -4758,7 +4758,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>46</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -4798,7 +4798,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>47</v>
       </c>
@@ -4821,7 +4821,7 @@
       <c r="G56" s="4"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>48</v>
       </c>
@@ -4844,40 +4844,62 @@
       <c r="G57" s="4"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="14"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
+        <v>49</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="10">
+        <v>1</v>
+      </c>
+      <c r="D58" s="10">
+        <v>1.5</v>
+      </c>
       <c r="E58" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F58" s="12"/>
+        <v>-0.3</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="G58" s="13"/>
-      <c r="H58" s="10"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E59" s="2">
-        <f>SUM(E16:E58)</f>
+      <c r="H58" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="2">
         <v>2.8</v>
       </c>
-      <c r="F59" s="2">
-        <f>COUNT(F16:F58)</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="2">
-        <f>COUNT(G16:G58)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F60" s="12">
+        <v>0</v>
+      </c>
+      <c r="G60" s="13">
+        <v>0</v>
+      </c>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>